<commit_message>
Generated BOM and Gerbers for v1.1
</commit_message>
<xml_diff>
--- a/manufacturing/ThreadSensorTag_BOM.xlsx
+++ b/manufacturing/ThreadSensorTag_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="nrf52-sensor-tag-v1.1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
-  <si>
-    <t>Reference</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+  <si>
+    <t>Reference(s)</t>
   </si>
   <si>
     <t>Qty</t>
@@ -43,45 +43,33 @@
     <t>BT1</t>
   </si>
   <si>
-    <t>Battery_Cell</t>
+    <t>SMTU2032-LF</t>
   </si>
   <si>
     <t>BA2032SM:BA2032SM</t>
   </si>
   <si>
-    <t>https://www.digikey.de/product-detail/en/mpd-memory-protection-devices/BA2032SM/BA2032SM-ND/257743</t>
-  </si>
-  <si>
-    <t>MPD (Memory Protection Devices)</t>
-  </si>
-  <si>
-    <t>BA2032SM</t>
-  </si>
-  <si>
-    <t>C3 C6</t>
-  </si>
-  <si>
-    <t>10uF</t>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Renata</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>0.22uF</t>
   </si>
   <si>
     <t>Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>C4 C7 C8</t>
+    <t>C7, C8</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>0.22uF</t>
-  </si>
-  <si>
     <t>IC2</t>
   </si>
   <si>
@@ -121,22 +109,28 @@
     <t>J3</t>
   </si>
   <si>
-    <t>Conn_01x07_Male</t>
-  </si>
-  <si>
     <t>Connector_PinHeader_2.54mm:PinHeader_1x07_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>JP1 JP2</t>
-  </si>
-  <si>
-    <t>SolderJumper_3_Bridged12</t>
-  </si>
-  <si>
-    <t>Jumper:SolderJumper-3_P1.3mm_Bridged12_RoundedPad1.0x1.5mm</t>
-  </si>
-  <si>
-    <t>R1 R2</t>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>APHF1608LSEEQBDZGKC</t>
+  </si>
+  <si>
+    <t>APHF1608LSEEQBDZGKC:APHF1608LSEEQBDZGKC</t>
+  </si>
+  <si>
+    <t>https://componentsearchengine.com/Datasheets/1/APHF1608LSEEQBDZGKC.pdf</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD RGB 0603 SMD</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
   </si>
   <si>
     <t>4.7k</t>
@@ -145,7 +139,7 @@
     <t>Resistor_SMD:R_0603_1608Metric</t>
   </si>
   <si>
-    <t>R3 R4</t>
+    <t>R3, R4</t>
   </si>
   <si>
     <t>10k</t>
@@ -154,10 +148,22 @@
     <t>R5</t>
   </si>
   <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>S1 S2</t>
+    <t>1k2</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>2k2</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>390R</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
   </si>
   <si>
     <t>EVQ-PUA02K</t>
@@ -182,13 +188,19 @@
   </si>
   <si>
     <t>MS88SF2:MS88SF2</t>
+  </si>
+  <si>
+    <t>https://www.minew.com/products/nrf52840-module-ms88sf2.html</t>
+  </si>
+  <si>
+    <t>Minew</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -200,25 +212,23 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+    </font>
+    <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,60 +241,35 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -295,7 +280,36 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8467725" cy="4581525"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.png" title="Bild"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,349 +516,363 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="5.0"/>
-    <col customWidth="1" min="3" max="3" width="28.57"/>
-    <col customWidth="1" min="4" max="4" width="35.14"/>
-    <col customWidth="1" min="5" max="5" width="6.14"/>
-    <col customWidth="1" min="8" max="8" width="22.29"/>
-    <col customWidth="1" min="9" max="9" width="29.29"/>
+    <col customWidth="1" min="2" max="2" width="5.29"/>
+    <col customWidth="1" min="3" max="3" width="29.71"/>
+    <col customWidth="1" min="4" max="4" width="34.71"/>
+    <col customWidth="1" min="5" max="5" width="7.0"/>
+    <col customWidth="1" min="8" max="8" width="26.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3">
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
         <v>2.0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="6" t="s">
+      <c r="B6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>24</v>
+      <c r="G6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6" t="s">
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="B8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4">
         <v>2.0</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4">
         <v>2.0</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="H14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="I14" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="5" t="s">
-        <v>55</v>
+      <c r="B15" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId1" ref="F5"/>
     <hyperlink r:id="rId2" ref="F6"/>
-    <hyperlink r:id="rId3" ref="F7"/>
-    <hyperlink r:id="rId4" ref="F13"/>
+    <hyperlink r:id="rId3" ref="F8"/>
+    <hyperlink r:id="rId4" ref="F14"/>
+    <hyperlink r:id="rId5" ref="F15"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>